<commit_message>
ajustes 1.0.1 (decimals salario,
</commit_message>
<xml_diff>
--- a/data/testes/funcionario.xlsx
+++ b/data/testes/funcionario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a-react\a - meus projetos\cydagReact\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a-react\a - meus projetos\cydag\data\testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774F1200-C048-4109-9ECD-F3BC622E7280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BF9506-DBA5-4D5A-85B0-49030DCDFA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>centroCusto</t>
   </si>
@@ -182,39 +182,6 @@
     <t>villhena clt temp</t>
   </si>
   <si>
-    <t>C0042TESTE </t>
-  </si>
-  <si>
-    <t>velho_01</t>
-  </si>
-  <si>
-    <t>velho_02</t>
-  </si>
-  <si>
-    <t>velho_03</t>
-  </si>
-  <si>
-    <t>velho_04</t>
-  </si>
-  <si>
-    <t>velho_05</t>
-  </si>
-  <si>
-    <t>velho_06</t>
-  </si>
-  <si>
-    <t>velho_07</t>
-  </si>
-  <si>
-    <t>velho_08</t>
-  </si>
-  <si>
-    <t>velho_09</t>
-  </si>
-  <si>
-    <t>0000DEPRE</t>
-  </si>
-  <si>
     <t>vaga1</t>
   </si>
   <si>
@@ -224,25 +191,16 @@
     <t>diretor</t>
   </si>
   <si>
-    <t>Paulo Ildefonso de Oliveira Cintra</t>
-  </si>
-  <si>
-    <t>analista de sistemas</t>
-  </si>
-  <si>
-    <t>velho_01a</t>
-  </si>
-  <si>
     <t>psicóloga</t>
   </si>
   <si>
     <t>gerente</t>
   </si>
   <si>
-    <t>idRH123</t>
-  </si>
-  <si>
     <t>idRh 12345</t>
+  </si>
+  <si>
+    <t>_TST1_CC10</t>
   </si>
 </sst>
 </file>
@@ -805,13 +763,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -854,13 +812,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -903,13 +861,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -952,13 +910,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1001,13 +959,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1050,13 +1008,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1099,13 +1057,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1148,13 +1106,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1197,13 +1155,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1542,11 +1500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,78 +1564,57 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="B2">
+        <v>123454</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F2">
-        <v>100000</v>
+        <v>1000</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>123455</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1000</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
       </c>
       <c r="K3" t="s">
         <v>37</v>
@@ -1688,16 +1625,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>1000</v>
@@ -1711,16 +1648,16 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>123457</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>1000</v>
@@ -1734,16 +1671,16 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>123458</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>1000</v>
@@ -1757,16 +1694,19 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="B7">
+        <v>123459</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
       </c>
       <c r="F7">
         <v>1000</v>
@@ -1780,19 +1720,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
         <v>59</v>
       </c>
+      <c r="B8">
+        <v>123460</v>
+      </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="F8">
         <v>1000</v>
@@ -1806,16 +1743,16 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="B9">
+        <v>123461</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>1000</v>
@@ -1829,65 +1766,42 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>123462</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
       </c>
       <c r="F10">
-        <v>1000</v>
+        <v>1000.34</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2000</v>
+      </c>
+      <c r="J10" t="s">
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11">
-        <v>1000</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>2000</v>
-      </c>
-      <c r="J11" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11">
         <v>4</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M10" t="s">
         <v>40</v>
       </c>
-      <c r="N11">
+      <c r="N10">
         <v>10</v>
       </c>
     </row>

</xml_diff>